<commit_message>
updated survay data format
</commit_message>
<xml_diff>
--- a/data/survay_data_modified.xlsx
+++ b/data/survay_data_modified.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ichih/Desktop/mcb536/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B656768-4194-4B4C-921D-D0D99B5C37AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A728F2F0-C110-AB40-999B-12E68078B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15580" xr2:uid="{BF7E64AF-ADBF-2D42-911C-688A4CE16EDF}"/>
   </bookViews>
   <sheets>
-    <sheet name="survay_data_test" sheetId="1" r:id="rId1"/>
+    <sheet name="survay_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="160" uniqueCount="19">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="160" uniqueCount="20">
   <si>
     <t>Field Season</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>calibrated</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -556,7 +559,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -579,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -1105,10 +1108,10 @@
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>13</v>
@@ -1197,10 +1200,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>15</v>
@@ -1243,10 +1246,10 @@
         <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
@@ -1361,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>13</v>
@@ -1381,13 +1384,13 @@
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>18</v>
@@ -1522,7 +1525,7 @@
         <v>9</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>8</v>

</xml_diff>